<commit_message>
correção de sensibilidade, reformulação de lógica, adição de plano VCC e atualização da BOM
</commit_message>
<xml_diff>
--- a/LOGICA NAO_BOM.xlsx
+++ b/LOGICA NAO_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>BOM LIST LOGICA NAO</t>
   </si>
@@ -31,12 +31,57 @@
     <t>CAPACITOR 100nF 0805</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C1, C2</t>
   </si>
   <si>
     <t>UMF212B7104KGHT, can be replaced to similar</t>
   </si>
   <si>
+    <t>RESISTOR 2.7K 0805</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RT0805FRE072K7L, can be replaced to similar</t>
+  </si>
+  <si>
+    <t>RESISTOR 510R 0806</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RT0805FRE07510RL, can be replaced to similar</t>
+  </si>
+  <si>
+    <t>RESISTOR 6.8K 0807</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RT0805FRE076K8L, can be replaced to similar</t>
+  </si>
+  <si>
+    <t>RESISTOR 10K 0808</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>RT0805FRE0710KL, can be replaced to similar</t>
+  </si>
+  <si>
+    <t>OPERACIONAL AMPLIFIER</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>LM358BIDR</t>
+  </si>
+  <si>
     <t>NAND SHCMITT TRIGGER</t>
   </si>
   <si>
@@ -44,15 +89,6 @@
   </si>
   <si>
     <t>74HC132D,653</t>
-  </si>
-  <si>
-    <t>OPERACIONAL AMPLIFIER</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>LM358BIDR</t>
   </si>
   <si>
     <t>MALE CONNECTOR</t>
@@ -404,7 +440,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -449,9 +485,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1564,7 +1597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1607,7 +1640,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s" s="10">
         <v>6</v>
@@ -1642,7 +1675,7 @@
       <c r="C5" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" t="s" s="11">
         <v>13</v>
       </c>
       <c r="E5" s="7"/>
@@ -1657,7 +1690,7 @@
       <c r="C6" t="s" s="14">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="14">
+      <c r="D6" t="s" s="11">
         <v>16</v>
       </c>
       <c r="E6" s="7"/>
@@ -1672,31 +1705,91 @@
       <c r="C7" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="D7" t="s" s="14">
-        <v>16</v>
+      <c r="D7" t="s" s="11">
+        <v>19</v>
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+    <row r="8" ht="17.05" customHeight="1">
+      <c r="A8" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+    <row r="9" ht="17.05" customHeight="1">
+      <c r="A9" t="s" s="12">
+        <v>23</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s" s="11">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+    <row r="10" ht="17.05" customHeight="1">
+      <c r="A10" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="14">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="17.05" customHeight="1">
+      <c r="A11" t="s" s="12">
+        <v>29</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="14">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>